<commit_message>
Feat: Adds multi currency to imports and exports (#89)
* Also adds ability for user to export configurations
</commit_message>
<xml_diff>
--- a/tests/0000_00_00_import_test.xlsx
+++ b/tests/0000_00_00_import_test.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coreyvarma/investbrain/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D52248-3C1D-564A-A6B2-79FD2F185FC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B60F390-F82C-4A49-9488-8DC485D816D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolios" sheetId="1" r:id="rId1"/>
     <sheet name="Transactions" sheetId="2" r:id="rId2"/>
     <sheet name="Daily Changes" sheetId="3" r:id="rId3"/>
+    <sheet name="Config" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Portfolio ID</t>
   </si>
@@ -106,6 +107,18 @@
   </si>
   <si>
     <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -502,15 +515,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -533,22 +546,25 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
@@ -564,11 +580,14 @@
       <c r="F2">
         <v>300</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -584,11 +603,14 @@
       <c r="F3">
         <v>200</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -604,9 +626,24 @@
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="K6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -618,7 +655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -652,4 +691,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D2BF26-877E-B64A-B037-8E1E4391E9EC}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>